<commit_message>
up to Images code
</commit_message>
<xml_diff>
--- a/Ivan_Product.xlsx
+++ b/Ivan_Product.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gautam.vavadiya\D\Personal\Jewel\Data_Extraction\Jewel_Data_Extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A40FF4-E433-4634-9E0E-4CF6B8DE1E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22911BA-28EC-4FEB-A27B-7D9C0F984E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{F5CA28F9-FEE6-4BC6-B3E3-F9ACA97D737E}"/>
   </bookViews>
@@ -701,7 +701,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>